<commit_message>
commit inclusión scripts de modelo operacional
</commit_message>
<xml_diff>
--- a/Estudio_Sensibilidades/Resultados_Energeticos_Sensibilidades.xlsx
+++ b/Estudio_Sensibilidades/Resultados_Energeticos_Sensibilidades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignac\Trabajo_Centra\Catedra-LDES\CII-Centra-EDF\SEN\SEN-Files\Electricity Generation\CII-CENTRA-EDF-CHILE\Estudio_Sensibilidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60867EF1-2DD9-40C2-AEFB-D04EF1A1016A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C47C390-585F-47C5-B716-E0F06C01EBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CasoBase" sheetId="1" r:id="rId1"/>
@@ -27,17 +27,28 @@
     <sheet name="PSP_2033" sheetId="12" r:id="rId12"/>
     <sheet name="Sin_PSP_10H" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="345">
   <si>
     <t>Capacidad instalada Generación</t>
   </si>
@@ -1021,6 +1032,57 @@
   </si>
   <si>
     <t>41.14</t>
+  </si>
+  <si>
+    <t>Capacidad instalada LDES (MW)</t>
+  </si>
+  <si>
+    <t>Capacidad instalada BESS (MW)</t>
+  </si>
+  <si>
+    <t>Capacidad instalada Generación (MW)</t>
+  </si>
+  <si>
+    <t>Participación renovable (%)</t>
+  </si>
+  <si>
+    <t>Participación renovable variable (%)</t>
+  </si>
+  <si>
+    <t>Solo viento y sol</t>
+  </si>
+  <si>
+    <t>Todo menos termicas</t>
+  </si>
+  <si>
+    <t>Generación bruta (GWh)</t>
+  </si>
+  <si>
+    <t>Energía movida por LDES (GWh)</t>
+  </si>
+  <si>
+    <t>Energía movida por BESS anual (GWh)</t>
+  </si>
+  <si>
+    <t>Participación renovable energía (%)</t>
+  </si>
+  <si>
+    <t>Participación renovable variable energía (%)</t>
+  </si>
+  <si>
+    <t>Recortes (GWh)</t>
+  </si>
+  <si>
+    <t>Energía no servida (GWh)</t>
+  </si>
+  <si>
+    <t>Generación bruta de 1 año del período</t>
+  </si>
+  <si>
+    <t>Energía inyectada por LDES</t>
+  </si>
+  <si>
+    <t>Energía inyectada por BESS anual</t>
   </si>
 </sst>
 </file>
@@ -1469,18 +1531,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J60"/>
+  <dimension ref="B2:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>45</v>
       </c>
@@ -1493,7 +1555,7 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
@@ -1508,7 +1570,7 @@
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
       <c r="C4" s="3">
         <v>2024</v>
@@ -1535,9 +1597,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="C5" s="7">
         <v>35819.81</v>
@@ -1564,9 +1626,9 @@
         <v>55246.36</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -1593,9 +1655,9 @@
         <v>4471.37</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>329</v>
       </c>
       <c r="C7" s="8">
         <v>387.5</v>
@@ -1622,9 +1684,9 @@
         <v>3419.69</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>331</v>
       </c>
       <c r="C8" s="8">
         <v>64.89</v>
@@ -1650,10 +1712,13 @@
       <c r="J8" s="8">
         <v>83.93</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>332</v>
       </c>
       <c r="C9" s="8">
         <v>41.3</v>
@@ -1679,10 +1744,13 @@
       <c r="J9" s="8">
         <v>68.17</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>335</v>
       </c>
       <c r="C10" s="8">
         <v>91340.26</v>
@@ -1708,10 +1776,13 @@
       <c r="J10" s="8">
         <v>133759.26</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>336</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -1737,10 +1808,13 @@
       <c r="J11" s="8">
         <v>12219.3</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>337</v>
       </c>
       <c r="C12" s="8">
         <v>637.16</v>
@@ -1766,10 +1840,13 @@
       <c r="J12" s="8">
         <v>5632.28</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>338</v>
       </c>
       <c r="C13" s="8">
         <v>66.72</v>
@@ -1796,9 +1873,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>339</v>
       </c>
       <c r="C14" s="8">
         <v>37.299999999999997</v>
@@ -1825,9 +1902,9 @@
         <v>67.739999999999995</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>340</v>
       </c>
       <c r="C15" s="8">
         <v>2108.42</v>
@@ -1854,7 +1931,7 @@
         <v>6326.07</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1885,7 +1962,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>341</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -1945,65 +2022,51 @@
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="9">
         <v>16528.5</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="9">
         <v>16770.599999999999</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6">
         <v>15413</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="9">
         <v>9000</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="9">
         <v>18088.2</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="9">
         <v>20144.900000000001</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="9">
         <v>8774.32</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="9">
         <v>8231.02</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="9">
-        <v>29.44</v>
-      </c>
-      <c r="D20" s="9">
-        <v>20.12</v>
-      </c>
-      <c r="E20" s="6">
-        <v>22.69</v>
-      </c>
-      <c r="F20" s="9">
-        <v>25.18</v>
-      </c>
-      <c r="G20" s="9">
-        <v>31.81</v>
-      </c>
-      <c r="H20" s="9">
-        <v>32.22</v>
-      </c>
-      <c r="I20" s="9">
-        <v>37.619999999999997</v>
-      </c>
-      <c r="J20" s="9">
-        <v>43.86</v>
-      </c>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="10"/>
+      <c r="B22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -2013,1041 +2076,968 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="3">
+        <v>2024</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2026</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2029</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2030</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2031</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2033</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2040</v>
+      </c>
+      <c r="J23" s="1">
+        <v>2050</v>
+      </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
-      <c r="C24" s="3">
-        <v>2024</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2026</v>
-      </c>
-      <c r="E24" s="1">
-        <v>2029</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2030</v>
-      </c>
-      <c r="G24" s="1">
-        <v>2031</v>
-      </c>
-      <c r="H24" s="1">
-        <v>2033</v>
-      </c>
-      <c r="I24" s="1">
-        <v>2040</v>
-      </c>
-      <c r="J24" s="1">
-        <v>2050</v>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <v>35819.81</v>
+      </c>
+      <c r="D24" s="7">
+        <v>41209.9</v>
+      </c>
+      <c r="E24" s="4">
+        <v>42543.97</v>
+      </c>
+      <c r="F24" s="7">
+        <v>44724.1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>45168.959999999999</v>
+      </c>
+      <c r="H24" s="7">
+        <v>47263.78</v>
+      </c>
+      <c r="I24" s="7">
+        <v>49299.9</v>
+      </c>
+      <c r="J24" s="7">
+        <v>59573.41</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="7">
-        <v>35819.81</v>
-      </c>
-      <c r="D25" s="7">
-        <v>41209.9</v>
-      </c>
-      <c r="E25" s="4">
-        <v>42543.97</v>
-      </c>
-      <c r="F25" s="7">
-        <v>44724.1</v>
-      </c>
-      <c r="G25" s="7">
-        <v>45168.959999999999</v>
-      </c>
-      <c r="H25" s="7">
-        <v>47263.78</v>
-      </c>
-      <c r="I25" s="7">
-        <v>49299.9</v>
-      </c>
-      <c r="J25" s="7">
-        <v>59573.41</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1420.22</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1470.75</v>
+      </c>
+      <c r="I25" s="8">
+        <v>1470.75</v>
+      </c>
+      <c r="J25" s="8">
+        <v>2557.04</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="8">
-        <v>0</v>
+        <v>387.5</v>
       </c>
       <c r="D26" s="8">
-        <v>0</v>
+        <v>2500.6</v>
       </c>
       <c r="E26" s="5">
-        <v>0</v>
+        <v>3128.55</v>
       </c>
       <c r="F26" s="8">
-        <v>0</v>
+        <v>3128.55</v>
       </c>
       <c r="G26" s="8">
-        <v>1420.22</v>
+        <v>3128.55</v>
       </c>
       <c r="H26" s="8">
-        <v>1470.75</v>
+        <v>3128.55</v>
       </c>
       <c r="I26" s="8">
-        <v>1470.75</v>
+        <v>4861.3</v>
       </c>
       <c r="J26" s="8">
-        <v>2557.04</v>
+        <v>8005.24</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="8">
-        <v>387.5</v>
+        <v>64.89</v>
       </c>
       <c r="D27" s="8">
-        <v>2500.6</v>
+        <v>69.209999999999994</v>
       </c>
       <c r="E27" s="5">
-        <v>3128.55</v>
+        <v>71.540000000000006</v>
       </c>
       <c r="F27" s="8">
-        <v>3128.55</v>
+        <v>73.239999999999995</v>
       </c>
       <c r="G27" s="8">
-        <v>3128.55</v>
+        <v>73.819999999999993</v>
       </c>
       <c r="H27" s="8">
-        <v>3128.55</v>
+        <v>74.98</v>
       </c>
       <c r="I27" s="8">
-        <v>4861.3</v>
+        <v>82.27</v>
       </c>
       <c r="J27" s="8">
-        <v>8005.24</v>
+        <v>85.32</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28" s="8">
-        <v>64.89</v>
+        <v>41.3</v>
       </c>
       <c r="D28" s="8">
-        <v>69.209999999999994</v>
+        <v>48.19</v>
       </c>
       <c r="E28" s="5">
-        <v>71.540000000000006</v>
+        <v>51.19</v>
       </c>
       <c r="F28" s="8">
-        <v>73.239999999999995</v>
+        <v>53.87</v>
       </c>
       <c r="G28" s="8">
-        <v>73.819999999999993</v>
+        <v>54.64</v>
       </c>
       <c r="H28" s="8">
-        <v>74.98</v>
+        <v>56.65</v>
       </c>
       <c r="I28" s="8">
-        <v>82.27</v>
+        <v>64.7</v>
       </c>
       <c r="J28" s="8">
-        <v>85.32</v>
+        <v>70.73</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" s="8">
-        <v>41.3</v>
+        <v>91982.64</v>
       </c>
       <c r="D29" s="8">
-        <v>48.19</v>
+        <v>96198.02</v>
       </c>
       <c r="E29" s="5">
-        <v>51.19</v>
+        <v>97937.49</v>
       </c>
       <c r="F29" s="8">
-        <v>53.87</v>
+        <v>98390.3</v>
       </c>
       <c r="G29" s="8">
-        <v>54.64</v>
+        <v>99753.97</v>
       </c>
       <c r="H29" s="8">
-        <v>56.65</v>
+        <v>101875.72</v>
       </c>
       <c r="I29" s="8">
-        <v>64.7</v>
+        <v>113943.12</v>
       </c>
       <c r="J29" s="8">
-        <v>70.73</v>
+        <v>134924.76999999999</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="8">
-        <v>91982.64</v>
+        <v>0</v>
       </c>
       <c r="D30" s="8">
-        <v>96198.02</v>
+        <v>0</v>
       </c>
       <c r="E30" s="5">
-        <v>97937.49</v>
+        <v>0</v>
       </c>
       <c r="F30" s="8">
-        <v>98390.3</v>
+        <v>0</v>
       </c>
       <c r="G30" s="8">
-        <v>99753.97</v>
+        <v>3968.11</v>
       </c>
       <c r="H30" s="8">
-        <v>101875.72</v>
+        <v>4130.66</v>
       </c>
       <c r="I30" s="8">
-        <v>113943.12</v>
+        <v>4268.72</v>
       </c>
       <c r="J30" s="8">
-        <v>134924.76999999999</v>
+        <v>6042.07</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" s="8">
-        <v>0</v>
+        <v>624.74</v>
       </c>
       <c r="D31" s="8">
-        <v>0</v>
+        <v>6030.48</v>
       </c>
       <c r="E31" s="5">
-        <v>0</v>
+        <v>6475.56</v>
       </c>
       <c r="F31" s="8">
-        <v>0</v>
+        <v>6218.7</v>
       </c>
       <c r="G31" s="8">
-        <v>3968.11</v>
+        <v>5386.09</v>
       </c>
       <c r="H31" s="8">
-        <v>4130.66</v>
+        <v>5454</v>
       </c>
       <c r="I31" s="8">
-        <v>4268.72</v>
+        <v>7958.39</v>
       </c>
       <c r="J31" s="8">
-        <v>6042.07</v>
+        <v>13052.06</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32" s="8">
-        <v>624.74</v>
+        <v>66.12</v>
       </c>
       <c r="D32" s="8">
-        <v>6030.48</v>
+        <v>75.260000000000005</v>
       </c>
       <c r="E32" s="5">
-        <v>6475.56</v>
+        <v>77.06</v>
       </c>
       <c r="F32" s="8">
-        <v>6218.7</v>
+        <v>83.76</v>
       </c>
       <c r="G32" s="8">
-        <v>5386.09</v>
+        <v>87.53</v>
       </c>
       <c r="H32" s="8">
-        <v>5454</v>
+        <v>90.43</v>
       </c>
       <c r="I32" s="8">
-        <v>7958.39</v>
+        <v>91.56</v>
       </c>
       <c r="J32" s="8">
-        <v>13052.06</v>
+        <v>93.37</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C33" s="8">
-        <v>66.12</v>
+        <v>36.81</v>
       </c>
       <c r="D33" s="8">
-        <v>75.260000000000005</v>
+        <v>47.32</v>
       </c>
       <c r="E33" s="5">
-        <v>77.06</v>
+        <v>52.01</v>
       </c>
       <c r="F33" s="8">
-        <v>83.76</v>
+        <v>57.68</v>
       </c>
       <c r="G33" s="8">
-        <v>87.53</v>
+        <v>61.13</v>
       </c>
       <c r="H33" s="8">
-        <v>90.43</v>
+        <v>65.16</v>
       </c>
       <c r="I33" s="8">
-        <v>91.56</v>
+        <v>68.959999999999994</v>
       </c>
       <c r="J33" s="8">
-        <v>93.37</v>
+        <v>74.87</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C34" s="8">
-        <v>36.81</v>
+        <v>2315.64</v>
       </c>
       <c r="D34" s="8">
-        <v>47.32</v>
+        <v>4138.7700000000004</v>
       </c>
       <c r="E34" s="5">
-        <v>52.01</v>
+        <v>3695.99</v>
       </c>
       <c r="F34" s="8">
-        <v>57.68</v>
+        <v>3663.76</v>
       </c>
       <c r="G34" s="8">
-        <v>61.13</v>
+        <v>2285.66</v>
       </c>
       <c r="H34" s="8">
-        <v>65.16</v>
+        <v>3881.59</v>
       </c>
       <c r="I34" s="8">
-        <v>68.959999999999994</v>
+        <v>4787.6099999999997</v>
       </c>
       <c r="J34" s="8">
-        <v>74.87</v>
+        <v>7670.38</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" s="8">
-        <v>2315.64</v>
+        <v>6.84</v>
       </c>
       <c r="D35" s="8">
-        <v>4138.7700000000004</v>
+        <v>9.09</v>
       </c>
       <c r="E35" s="5">
-        <v>3695.99</v>
+        <v>7.26</v>
       </c>
       <c r="F35" s="8">
-        <v>3663.76</v>
+        <v>6.46</v>
       </c>
       <c r="G35" s="8">
-        <v>2285.66</v>
+        <v>3.75</v>
       </c>
       <c r="H35" s="8">
-        <v>3881.59</v>
+        <v>5.85</v>
       </c>
       <c r="I35" s="8">
-        <v>4787.6099999999997</v>
+        <v>6.09</v>
       </c>
       <c r="J35" s="8">
-        <v>7670.38</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C36" s="8">
-        <v>6.84</v>
+        <v>0</v>
       </c>
       <c r="D36" s="8">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="E36" s="5">
-        <v>7.26</v>
+        <v>0</v>
       </c>
       <c r="F36" s="8">
-        <v>6.46</v>
+        <v>0</v>
       </c>
       <c r="G36" s="8">
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="H36" s="8">
-        <v>5.85</v>
+        <v>0</v>
       </c>
       <c r="I36" s="8">
-        <v>6.09</v>
+        <v>0</v>
       </c>
       <c r="J36" s="8">
-        <v>7.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" s="8">
-        <v>0</v>
+        <v>81640.2</v>
       </c>
       <c r="D37" s="8">
-        <v>0</v>
+        <v>82935.649999999994</v>
       </c>
       <c r="E37" s="5">
-        <v>0</v>
+        <v>84435.02</v>
       </c>
       <c r="F37" s="8">
-        <v>0</v>
+        <v>84877.46</v>
       </c>
       <c r="G37" s="8">
-        <v>0</v>
+        <v>86608.24</v>
       </c>
       <c r="H37" s="8">
-        <v>0</v>
+        <v>89386.5</v>
       </c>
       <c r="I37" s="8">
-        <v>0</v>
+        <v>99877.59</v>
       </c>
       <c r="J37" s="8">
-        <v>0</v>
+        <v>116501.8</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="8">
-        <v>81640.2</v>
-      </c>
-      <c r="D38" s="8">
-        <v>82935.649999999994</v>
-      </c>
-      <c r="E38" s="5">
-        <v>84435.02</v>
-      </c>
-      <c r="F38" s="8">
-        <v>84877.46</v>
-      </c>
-      <c r="G38" s="8">
-        <v>86608.24</v>
-      </c>
-      <c r="H38" s="8">
-        <v>89386.5</v>
-      </c>
-      <c r="I38" s="8">
-        <v>99877.59</v>
-      </c>
-      <c r="J38" s="8">
-        <v>116501.8</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C38" s="9">
         <v>16528.5</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D38" s="9">
         <v>16770.599999999999</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E38" s="6">
         <v>15413</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F38" s="9">
         <v>6421.07</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G38" s="9">
         <v>4299.78</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H38" s="9">
         <v>3433.05</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I38" s="9">
         <v>3344.12</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J38" s="9">
         <v>3403.02</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="9">
-        <v>33.71</v>
-      </c>
-      <c r="D40" s="9">
-        <v>24.01</v>
-      </c>
-      <c r="E40" s="6">
-        <v>26.64</v>
-      </c>
-      <c r="F40" s="9">
-        <v>28.98</v>
-      </c>
-      <c r="G40" s="9">
-        <v>35.44</v>
-      </c>
-      <c r="H40" s="9">
-        <v>35.19</v>
-      </c>
-      <c r="I40" s="9">
-        <v>38.520000000000003</v>
-      </c>
-      <c r="J40" s="9">
-        <v>42.81</v>
-      </c>
+      <c r="B40" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B42" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="3">
+        <v>2024</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2026</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2029</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2030</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2031</v>
+      </c>
+      <c r="H42" s="1">
+        <v>2033</v>
+      </c>
+      <c r="I42" s="1">
+        <v>2040</v>
+      </c>
+      <c r="J42" s="1">
+        <v>2050</v>
+      </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
+      <c r="B43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="7">
+        <v>35819.81</v>
+      </c>
+      <c r="D43" s="7">
+        <v>41150.54</v>
+      </c>
+      <c r="E43" s="4">
+        <v>43525.56</v>
+      </c>
+      <c r="F43" s="7">
+        <v>42167.61</v>
+      </c>
+      <c r="G43" s="7">
+        <v>42760.82</v>
+      </c>
+      <c r="H43" s="7">
+        <v>45267.19</v>
+      </c>
+      <c r="I43" s="7">
+        <v>51181.02</v>
+      </c>
+      <c r="J43" s="7">
+        <v>63230.080000000002</v>
+      </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="11"/>
-      <c r="C44" s="3">
-        <v>2024</v>
-      </c>
-      <c r="D44" s="1">
-        <v>2026</v>
-      </c>
-      <c r="E44" s="1">
-        <v>2029</v>
-      </c>
-      <c r="F44" s="1">
-        <v>2030</v>
-      </c>
-      <c r="G44" s="1">
-        <v>2031</v>
-      </c>
-      <c r="H44" s="1">
-        <v>2033</v>
-      </c>
-      <c r="I44" s="1">
-        <v>2040</v>
-      </c>
-      <c r="J44" s="1">
-        <v>2050</v>
+      <c r="B44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8">
+        <v>0</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0</v>
+      </c>
+      <c r="G44" s="8">
+        <v>1461.83</v>
+      </c>
+      <c r="H44" s="8">
+        <v>1462.9</v>
+      </c>
+      <c r="I44" s="8">
+        <v>1462.9</v>
+      </c>
+      <c r="J44" s="8">
+        <v>2092.8200000000002</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="7">
-        <v>35819.81</v>
-      </c>
-      <c r="D45" s="7">
-        <v>41150.54</v>
-      </c>
-      <c r="E45" s="4">
-        <v>43525.56</v>
-      </c>
-      <c r="F45" s="7">
-        <v>42167.61</v>
-      </c>
-      <c r="G45" s="7">
-        <v>42760.82</v>
-      </c>
-      <c r="H45" s="7">
-        <v>45267.19</v>
-      </c>
-      <c r="I45" s="7">
-        <v>51181.02</v>
-      </c>
-      <c r="J45" s="7">
-        <v>63230.080000000002</v>
+        <v>2</v>
+      </c>
+      <c r="C45" s="8">
+        <v>387.5</v>
+      </c>
+      <c r="D45" s="8">
+        <v>2632.18</v>
+      </c>
+      <c r="E45" s="5">
+        <v>3641.02</v>
+      </c>
+      <c r="F45" s="8">
+        <v>3641.02</v>
+      </c>
+      <c r="G45" s="8">
+        <v>3641.02</v>
+      </c>
+      <c r="H45" s="8">
+        <v>3694.03</v>
+      </c>
+      <c r="I45" s="8">
+        <v>4845.4399999999996</v>
+      </c>
+      <c r="J45" s="8">
+        <v>10018.31</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C46" s="8">
-        <v>0</v>
+        <v>64.89</v>
       </c>
       <c r="D46" s="8">
-        <v>0</v>
+        <v>69.17</v>
       </c>
       <c r="E46" s="5">
-        <v>0</v>
+        <v>72.19</v>
       </c>
       <c r="F46" s="8">
-        <v>0</v>
+        <v>79.27</v>
       </c>
       <c r="G46" s="8">
-        <v>1461.83</v>
+        <v>79.55</v>
       </c>
       <c r="H46" s="8">
-        <v>1462.9</v>
+        <v>80.69</v>
       </c>
       <c r="I46" s="8">
-        <v>1462.9</v>
+        <v>82.92</v>
       </c>
       <c r="J46" s="8">
-        <v>2092.8200000000002</v>
+        <v>86.17</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C47" s="8">
-        <v>387.5</v>
+        <v>41.3</v>
       </c>
       <c r="D47" s="8">
-        <v>2632.18</v>
+        <v>48.12</v>
       </c>
       <c r="E47" s="5">
-        <v>3641.02</v>
+        <v>52.29</v>
       </c>
       <c r="F47" s="8">
-        <v>3641.02</v>
+        <v>58.71</v>
       </c>
       <c r="G47" s="8">
-        <v>3641.02</v>
+        <v>59.28</v>
       </c>
       <c r="H47" s="8">
-        <v>3694.03</v>
+        <v>61.53</v>
       </c>
       <c r="I47" s="8">
-        <v>4845.4399999999996</v>
+        <v>65.98</v>
       </c>
       <c r="J47" s="8">
-        <v>10018.31</v>
+        <v>72.3</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C48" s="8">
-        <v>64.89</v>
+        <v>91174.04</v>
       </c>
       <c r="D48" s="8">
-        <v>69.17</v>
+        <v>94965.9</v>
       </c>
       <c r="E48" s="5">
-        <v>72.19</v>
+        <v>95874.02</v>
       </c>
       <c r="F48" s="8">
-        <v>79.27</v>
+        <v>95900.41</v>
       </c>
       <c r="G48" s="8">
-        <v>79.55</v>
+        <v>97412.29</v>
       </c>
       <c r="H48" s="8">
-        <v>80.69</v>
+        <v>100152.16</v>
       </c>
       <c r="I48" s="8">
-        <v>82.92</v>
+        <v>114143.74</v>
       </c>
       <c r="J48" s="8">
-        <v>86.17</v>
+        <v>139058.82999999999</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C49" s="8">
-        <v>41.3</v>
+        <v>0</v>
       </c>
       <c r="D49" s="8">
-        <v>48.12</v>
+        <v>0</v>
       </c>
       <c r="E49" s="5">
-        <v>52.29</v>
+        <v>0</v>
       </c>
       <c r="F49" s="8">
-        <v>58.71</v>
+        <v>0</v>
       </c>
       <c r="G49" s="8">
-        <v>59.28</v>
+        <v>4043.38</v>
       </c>
       <c r="H49" s="8">
-        <v>61.53</v>
+        <v>4245.46</v>
       </c>
       <c r="I49" s="8">
-        <v>65.98</v>
+        <v>4262.57</v>
       </c>
       <c r="J49" s="8">
-        <v>72.3</v>
+        <v>4328.33</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50" s="8">
-        <v>91174.04</v>
+        <v>641.98</v>
       </c>
       <c r="D50" s="8">
-        <v>94965.9</v>
+        <v>6248.89</v>
       </c>
       <c r="E50" s="5">
-        <v>95874.02</v>
+        <v>7521.79</v>
       </c>
       <c r="F50" s="8">
-        <v>95900.41</v>
+        <v>7191.88</v>
       </c>
       <c r="G50" s="8">
-        <v>97412.29</v>
+        <v>6348.78</v>
       </c>
       <c r="H50" s="8">
-        <v>100152.16</v>
+        <v>6703.74</v>
       </c>
       <c r="I50" s="8">
-        <v>114143.74</v>
+        <v>8812.2800000000007</v>
       </c>
       <c r="J50" s="8">
-        <v>139058.82999999999</v>
+        <v>17331.32</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C51" s="8">
-        <v>0</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="D51" s="8">
-        <v>0</v>
+        <v>76.28</v>
       </c>
       <c r="E51" s="5">
-        <v>0</v>
+        <v>81.28</v>
       </c>
       <c r="F51" s="8">
-        <v>0</v>
+        <v>86.92</v>
       </c>
       <c r="G51" s="8">
-        <v>4043.38</v>
+        <v>90.68</v>
       </c>
       <c r="H51" s="8">
-        <v>4245.46</v>
+        <v>93.72</v>
       </c>
       <c r="I51" s="8">
-        <v>4262.57</v>
+        <v>94.22</v>
       </c>
       <c r="J51" s="8">
-        <v>4328.33</v>
+        <v>95.76</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C52" s="8">
-        <v>641.98</v>
+        <v>37.19</v>
       </c>
       <c r="D52" s="8">
-        <v>6248.89</v>
+        <v>48.12</v>
       </c>
       <c r="E52" s="5">
-        <v>7521.79</v>
+        <v>55.7</v>
       </c>
       <c r="F52" s="8">
-        <v>7191.88</v>
+        <v>60.38</v>
       </c>
       <c r="G52" s="8">
-        <v>6348.78</v>
+        <v>63.96</v>
       </c>
       <c r="H52" s="8">
-        <v>6703.74</v>
+        <v>68.39</v>
       </c>
       <c r="I52" s="8">
-        <v>8812.2800000000007</v>
+        <v>72.25</v>
       </c>
       <c r="J52" s="8">
-        <v>17331.32</v>
+        <v>78.06</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C53" s="8">
-        <v>66.599999999999994</v>
+        <v>2286.35</v>
       </c>
       <c r="D53" s="8">
-        <v>76.28</v>
+        <v>3842.88</v>
       </c>
       <c r="E53" s="5">
-        <v>81.28</v>
+        <v>4094.35</v>
       </c>
       <c r="F53" s="8">
-        <v>86.92</v>
+        <v>4452.47</v>
       </c>
       <c r="G53" s="8">
-        <v>90.68</v>
+        <v>2867.65</v>
       </c>
       <c r="H53" s="8">
-        <v>93.72</v>
+        <v>4919.9799999999996</v>
       </c>
       <c r="I53" s="8">
-        <v>94.22</v>
+        <v>6254.8</v>
       </c>
       <c r="J53" s="8">
-        <v>95.76</v>
+        <v>9827.07</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C54" s="8">
-        <v>37.19</v>
+        <v>6.74</v>
       </c>
       <c r="D54" s="8">
-        <v>48.12</v>
+        <v>8.41</v>
       </c>
       <c r="E54" s="5">
-        <v>55.7</v>
+        <v>7.67</v>
       </c>
       <c r="F54" s="8">
-        <v>60.38</v>
+        <v>7.69</v>
       </c>
       <c r="G54" s="8">
-        <v>63.96</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H54" s="8">
-        <v>68.39</v>
+        <v>7.18</v>
       </c>
       <c r="I54" s="8">
-        <v>72.25</v>
+        <v>7.58</v>
       </c>
       <c r="J54" s="8">
-        <v>78.06</v>
+        <v>9.0500000000000007</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C55" s="8">
-        <v>2286.35</v>
+        <v>0</v>
       </c>
       <c r="D55" s="8">
-        <v>3842.88</v>
+        <v>0</v>
       </c>
       <c r="E55" s="5">
-        <v>4094.35</v>
+        <v>0</v>
       </c>
       <c r="F55" s="8">
-        <v>4452.47</v>
+        <v>0</v>
       </c>
       <c r="G55" s="8">
-        <v>2867.65</v>
+        <v>0</v>
       </c>
       <c r="H55" s="8">
-        <v>4919.9799999999996</v>
+        <v>0</v>
       </c>
       <c r="I55" s="8">
-        <v>6254.8</v>
+        <v>0</v>
       </c>
       <c r="J55" s="8">
-        <v>9827.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C56" s="8">
-        <v>6.74</v>
+        <v>80571.92</v>
       </c>
       <c r="D56" s="8">
-        <v>8.41</v>
+        <v>81203.67</v>
       </c>
       <c r="E56" s="5">
-        <v>7.67</v>
+        <v>82018</v>
       </c>
       <c r="F56" s="8">
-        <v>7.69</v>
+        <v>82130.59</v>
       </c>
       <c r="G56" s="8">
-        <v>4.5999999999999996</v>
+        <v>83804.350000000006</v>
       </c>
       <c r="H56" s="8">
-        <v>7.18</v>
+        <v>86876.39</v>
       </c>
       <c r="I56" s="8">
-        <v>7.58</v>
+        <v>98999.14</v>
       </c>
       <c r="J56" s="8">
-        <v>9.0500000000000007</v>
+        <v>118527.63</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="8">
-        <v>0</v>
-      </c>
-      <c r="D57" s="8">
-        <v>0</v>
-      </c>
-      <c r="E57" s="5">
-        <v>0</v>
-      </c>
-      <c r="F57" s="8">
-        <v>0</v>
-      </c>
-      <c r="G57" s="8">
-        <v>0</v>
-      </c>
-      <c r="H57" s="8">
-        <v>0</v>
-      </c>
-      <c r="I57" s="8">
-        <v>0</v>
-      </c>
-      <c r="J57" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="8">
-        <v>80571.92</v>
-      </c>
-      <c r="D58" s="8">
-        <v>81203.67</v>
-      </c>
-      <c r="E58" s="5">
-        <v>82018</v>
-      </c>
-      <c r="F58" s="8">
-        <v>82130.59</v>
-      </c>
-      <c r="G58" s="8">
-        <v>83804.350000000006</v>
-      </c>
-      <c r="H58" s="8">
-        <v>86876.39</v>
-      </c>
-      <c r="I58" s="8">
-        <v>98999.14</v>
-      </c>
-      <c r="J58" s="8">
-        <v>118527.63</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C57" s="9">
         <v>16528.5</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D57" s="9">
         <v>16255.5</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E57" s="6">
         <v>12436.9</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F57" s="9">
         <v>4615.8900000000003</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G57" s="9">
         <v>3091.29</v>
       </c>
-      <c r="H59" s="8">
+      <c r="H57" s="9">
         <v>2155.2600000000002</v>
       </c>
-      <c r="I59" s="8">
+      <c r="I57" s="9">
         <v>2243.64</v>
       </c>
-      <c r="J59" s="8">
+      <c r="J57" s="9">
         <v>2194.96</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B60" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="9">
-        <v>35.56</v>
-      </c>
-      <c r="D60" s="9">
-        <v>25.31</v>
-      </c>
-      <c r="E60" s="6">
-        <v>26.84</v>
-      </c>
-      <c r="F60" s="9">
-        <v>27.88</v>
-      </c>
-      <c r="G60" s="9">
-        <v>34.33</v>
-      </c>
-      <c r="H60" s="9">
-        <v>33.58</v>
-      </c>
-      <c r="I60" s="9">
-        <v>37.11</v>
-      </c>
-      <c r="J60" s="9">
-        <v>41.41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:J41"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="B40:J40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3057,11 +3047,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FF3032-6E37-46D8-B420-078FD3E1A2AB}">
   <dimension ref="B2:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -4645,6 +4638,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -6228,6 +6224,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -7811,6 +7810,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -16807,11 +16809,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C564DC6D-B371-4D56-9CDF-96B810FDA092}">
   <dimension ref="B2:J60"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -18395,6 +18400,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -19978,6 +19986,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">

</xml_diff>